<commit_message>
Errores en preciarios generales
</commit_message>
<xml_diff>
--- a/OSEF.ERP.APP/preciariosGenerales/MnttoMediaPrueba.xlsx
+++ b/OSEF.ERP.APP/preciariosGenerales/MnttoMediaPrueba.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osef\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1038,6 +1038,9 @@
     <t xml:space="preserve">SUMINISTRO DE UNIDAD DE AIRE ACONDICIONADO TIPO DIVIDIDO DE EXPANSIÓN DIRECTA CONSISTENTE EN UNIDAD EVAPORADORA TIPO FAN &amp; COIL CAPACIDAD NOMINAL DE 18, 000 BTU/HR, CERTIFICACIÓN ARI, CONTROLADOR ELECTRÓNICO DE PROTOCOLO ABIERTO PARA ENLACE CON SISTEMA DE AUTOMATIZACIÓN, TRES HILERAS, PARA MANEJAR 600 CFM, REFRIGERANTE R-410A CON MOTOR A 220V-1FASES-60HZ, CAJA PLENUM, FILTRO METÁLICO LAVABLE INCLUIDO, Y UNIDAD CONDENSADORA SOLO FRIO CAPACIDAD NOMINAL DE 18, 000 BTU/HR, CERTIFICACIÓN ARI, CONTROLADOR ELECTRÓNICO DE PROTOCOLO ABIERTO PARA ENLACE CON SISTEMA DE AUTOMATIZACIÓN, COMPRESOR SCROLL, EFICIENCIA 13 SEER REFRIGERANTE R-410A PARA OPERAR A 220V-1FASE-60HZ CON PROTECCIÓN ANTICORROSIVA. </t>
   </si>
   <si>
+    <t>=</t>
+  </si>
+  <si>
     <t xml:space="preserve">SUMINISTRO DE UNIDAD DE AIRE ACONDICIONADO TIPO DIVIDIDO DE EXPANSIÓN DIRECTA CONSISTENTE EN UNIDAD EVAPORADORA TIPO FAN &amp; COIL CAPACIDAD NOMINAL DE 24, 000 BTU/HR, CERTIFICACIÓN ARI, CONTROLADOR ELECTRÓNICO DE PROTOCOLO ABIERTO PARA ENLACE CON SISTEMA DE AUTOMATIZACIÓN, TRES HILERAS, PARA MANEJAR 800 CFM, REFRIGERANTE R-410A CON MOTOR A 220V-1FASES-60HZ, CAJA PLENUM, FILTRO METÁLICO LAVABLE INCLUIDO, Y UNIDAD CONDENSADORA SOLO FRIO CAPACIDAD NOMINAL DE 24, 000 BTU/HR, CERTIFICACIÓN ARI, CONTROLADOR ELECTRÓNICO DE PROTOCOLO ABIERTO PARA ENLACE CON SISTEMA DE AUTOMATIZACIÓN, COMPRESOR SCROLL, EFICIENCIA 13 SEER REFRIGERANTE R-410A PARA OPERAR A 220V-1FASE-60HZ CON PROTECCIÓN ANTICORROSIVA. </t>
   </si>
   <si>
@@ -1057,9 +1060,6 @@
   </si>
   <si>
     <t xml:space="preserve">SUMINISTRO DE UNIDAD DE AIRE ACONDICIONADO TIPO DIVIDIDO DE EXPANSIÓN DIRECTA CONSISTENTE EN UNIDAD EVAPORADORA TIPO FAN &amp; COIL CAPACIDAD NOMINAL DE 48, 000 BTU/HR, CERTIFICACIÓN ARI, CONTROLADOR ELECTRÓNICO DE PROTOCOLO ABIERTO PARA ENLACE CON SISTEMA DE AUTOMATIZACIÓN, TRES HILERAS, PARA MANEJAR 1, 600 CFM, REFRIGERANTE R-410A CON MOTOR A 220V-1FASES-60HZ, CAJA PLENUM, FILTRO METÁLICO LAVABLE INCLUIDO, Y UNIDAD CONDENSADORA SOLO FRIO CAPACIDAD NOMINAL DE 48, 000 BTU/HR, CERTIFICACIÓN ARI, CONTROLADOR ELECTRÓNICO DE PROTOCOLO ABIERTO PARA ENLACE CON SISTEMA DE AUTOMATIZACIÓN, COMPRESOR SCROLL, EFICIENCIA 13 SEER REFRIGERANTE R-410A PARA OPERAR A 220V-3FASES-60HZ CON PROTECCIÓN ANTICORROSIVA. </t>
-  </si>
-  <si>
-    <t>DAA-138</t>
   </si>
 </sst>
 </file>
@@ -1726,7 +1726,7 @@
   <dimension ref="A1:G164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A162" sqref="A162"/>
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4148,10 +4148,10 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="53" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="B161" s="54" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C161" s="55" t="s">
         <v>15</v>
@@ -4166,10 +4166,10 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="53" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B162" s="54" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C162" s="55" t="s">
         <v>15</v>
@@ -4184,10 +4184,10 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="53" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B163" s="54" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C163" s="55" t="s">
         <v>15</v>
@@ -4202,10 +4202,10 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="53" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B164" s="54" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C164" s="55" t="s">
         <v>15</v>

</xml_diff>